<commit_message>
parsing data from excel with Pandas
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cosyma\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cosyma_lab\PycharmProjects\TestP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="13905" windowHeight="12465"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="13905" windowHeight="12465"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>x</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>m</t>
+  </si>
+  <si>
+    <t>weight</t>
   </si>
 </sst>
 </file>
@@ -361,15 +364,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -379,8 +382,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -390,8 +396,11 @@
       <c r="C2">
         <v>65</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>79.599999999999994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -401,8 +410,11 @@
       <c r="C3">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>79.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>76</v>
       </c>
@@ -412,8 +424,11 @@
       <c r="C4">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>79.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>34</v>
       </c>
@@ -423,8 +438,11 @@
       <c r="C5">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>79.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>27</v>
       </c>
@@ -434,8 +452,11 @@
       <c r="C6">
         <v>87</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>79.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>56</v>
       </c>
@@ -445,8 +466,11 @@
       <c r="C7">
         <v>56</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>79.400000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
@@ -456,8 +480,11 @@
       <c r="C8">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>79.599999999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>46</v>
       </c>
@@ -467,8 +494,11 @@
       <c r="C9">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>79.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -478,8 +508,11 @@
       <c r="C10">
         <v>65</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>79.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>54</v>
       </c>
@@ -489,8 +522,11 @@
       <c r="C11">
         <v>89</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>79.400000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>87</v>
       </c>
@@ -500,8 +536,11 @@
       <c r="C12">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>79.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -511,8 +550,11 @@
       <c r="C13">
         <v>65</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>79.400000000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>23</v>
       </c>
@@ -522,8 +564,11 @@
       <c r="C14">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>79.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -533,8 +578,11 @@
       <c r="C15">
         <v>87</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>79.099999999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>54</v>
       </c>
@@ -544,8 +592,11 @@
       <c r="C16">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>23</v>
       </c>
@@ -555,8 +606,11 @@
       <c r="C17">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>78.900000000000006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>65</v>
       </c>
@@ -566,8 +620,11 @@
       <c r="C18">
         <v>76</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>78.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>34</v>
       </c>
@@ -577,8 +634,11 @@
       <c r="C19">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>78.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>76</v>
       </c>
@@ -588,8 +648,11 @@
       <c r="C20">
         <v>77</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>78.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>98</v>
       </c>
@@ -599,8 +662,11 @@
       <c r="C21">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>78.599999999999994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>23</v>
       </c>
@@ -609,6 +675,17 @@
       </c>
       <c r="C22">
         <v>32</v>
+      </c>
+      <c r="E22">
+        <v>78.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>32</v>
+      </c>
+      <c r="E23">
+        <v>78.599999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>